<commit_message>
adding avg number of words per sentence
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Categorized Records.xlsx
+++ b/Dataset Excel Sheets/Categorized Records.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/080c280c8b6910c1/Desktop/AUS/4. Senior Year/Spring 2024/Senior Design II/Senior-Design-Code/Dataset Excel Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_0A6555895B00520CAF1B3611595ED87656CDCF99" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBC664F0-17BA-439A-90D1-38FCE62102BF}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_0A6555895B00520CAF1B3611595ED87656CDCF99" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A63A3E63-8E70-4BCB-9650-6B7C23598CF8}"/>
   <bookViews>
-    <workbookView xWindow="264" yWindow="180" windowWidth="22776" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="264" yWindow="96" windowWidth="21732" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Sentence</t>
   </si>
@@ -329,6 +342,9 @@
   </si>
   <si>
     <t>[50]</t>
+  </si>
+  <si>
+    <t>Average Number of Words Per Sentence</t>
   </si>
 </sst>
 </file>
@@ -384,11 +400,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,6 +421,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -691,15 +712,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1262,6 +1284,15 @@
       </c>
       <c r="C51">
         <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="2">
+        <f>SUM(C2:C51)/50</f>
+        <v>3.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 02-Saving Frames Statistics
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Categorized Records.xlsx
+++ b/Dataset Excel Sheets/Categorized Records.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/080c280c8b6910c1/Desktop/AUS/4. Senior Year/Spring 2024/Senior Design II/Senior-Design-Code/Dataset Excel Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaher.salman\Desktop\LINA JAN 24\Senior II\Senior-Design-Code\Dataset Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_0A6555895B00520CAF1B3611595ED87656CDCF99" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A63A3E63-8E70-4BCB-9650-6B7C23598CF8}"/>
   <bookViews>
-    <workbookView xWindow="264" yWindow="96" windowWidth="21732" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="100" windowWidth="21730" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -350,7 +349,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -711,21 +710,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -736,7 +735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -747,7 +746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -758,7 +757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -769,7 +768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -780,7 +779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -791,7 +790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -802,7 +801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -813,7 +812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -824,7 +823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -835,7 +834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -846,7 +845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -857,7 +856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -868,7 +867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -879,7 +878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -890,7 +889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>89</v>
       </c>
@@ -901,7 +900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -912,7 +911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -923,7 +922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -934,7 +933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -945,7 +944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -956,7 +955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -967,7 +966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -978,7 +977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -989,7 +988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1000,7 +999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1011,7 +1010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1022,7 +1021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -1033,7 +1032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -1044,7 +1043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -1055,7 +1054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -1066,7 +1065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -1077,7 +1076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -1088,7 +1087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>101</v>
       </c>
@@ -1110,7 +1109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1121,7 +1120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -1132,7 +1131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1143,7 +1142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1154,7 +1153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>59</v>
       </c>
@@ -1165,7 +1164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>61</v>
       </c>
@@ -1176,7 +1175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>65</v>
       </c>
@@ -1187,7 +1186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>95</v>
       </c>
@@ -1198,7 +1197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -1209,7 +1208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -1220,7 +1219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -1231,7 +1230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -1242,7 +1241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1253,7 +1252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -1264,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1275,7 +1274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -1286,17 +1285,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B54" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C54" s="2">
-        <f>SUM(C2:C51)/50</f>
+        <f>AVERAGE(C2:C51)</f>
         <v>3.1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C51">
+  <sortState ref="A2:C51">
     <sortCondition ref="C1:C51"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>